<commit_message>
Atualizacoes e criacao tela LOGIN
</commit_message>
<xml_diff>
--- a/documentacao/Planilha_De_Requisitos.xlsx
+++ b/documentacao/Planilha_De_Requisitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="5_{934F93CA-D754-4E8E-914F-610C2E6609FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBCB369-7DD0-4E5D-A257-434A3DAA0F44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -278,18 +278,18 @@
     <t>ATIVIDADE</t>
   </si>
   <si>
+    <t>Cadasrar login e senha no banco de dados</t>
+  </si>
+  <si>
+    <t>Gerar login e senha automaticamente</t>
+  </si>
+  <si>
+    <t>Validar login e senha via banco de dados</t>
+  </si>
+  <si>
     <t>Criar tela de login e senha</t>
   </si>
   <si>
-    <t>Cadasrar login e senha no banco de dados</t>
-  </si>
-  <si>
-    <t>Gerar login e senha automaticamente</t>
-  </si>
-  <si>
-    <t>Validar login e senha via banco de dados</t>
-  </si>
-  <si>
     <t>Alteração de Perfil</t>
   </si>
   <si>
@@ -302,12 +302,12 @@
     <t>Banco de Dados</t>
   </si>
   <si>
+    <t>Criação do Banco de Dados em Azure</t>
+  </si>
+  <si>
     <t>Modelagem de Banco de Dados</t>
   </si>
   <si>
-    <t>Criação do Banco de Dados em Azure</t>
-  </si>
-  <si>
     <t>Criação de Tabelas do Banco de Dados</t>
   </si>
   <si>
@@ -326,12 +326,12 @@
     <t>Montar a solução</t>
   </si>
   <si>
+    <t>Con. Com o banco de dados para armazenar os dados recolhidos</t>
+  </si>
+  <si>
     <t>Programar para manter a temperatura e umidade nos niveis ideias</t>
   </si>
   <si>
-    <t>Con. Com o banco de dados para armazenar os dados recolhidos</t>
-  </si>
-  <si>
     <t>Sites</t>
   </si>
   <si>
@@ -348,13 +348,16 @@
   </si>
   <si>
     <t>Graficos e Analtics</t>
+  </si>
+  <si>
+    <t>Total horas gastas:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,15 +409,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -432,8 +428,31 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -562,128 +581,43 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -694,7 +628,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -707,7 +641,35 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -716,14 +678,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
@@ -752,53 +805,116 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="7" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
-    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
-    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+  <cellStyles count="8">
+    <cellStyle name="20% - Ênfase2" xfId="7" builtinId="34"/>
+    <cellStyle name="40% - Ênfase1" xfId="3" builtinId="31"/>
+    <cellStyle name="40% - Ênfase2" xfId="5" builtinId="35"/>
+    <cellStyle name="60% - Ênfase2" xfId="6" builtinId="36"/>
+    <cellStyle name="Ênfase1" xfId="2" builtinId="29"/>
+    <cellStyle name="Ênfase2" xfId="4" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título 2" xfId="1" builtinId="17"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -882,13 +998,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -905,6 +1014,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -947,7 +1063,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:D10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="3"/>
@@ -960,7 +1076,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1258,11 +1374,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
@@ -1272,7 +1388,7 @@
     <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1288,7 +1404,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1302,7 +1418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1316,7 +1432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1330,7 +1446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1344,7 +1460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1358,7 +1474,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1372,7 +1488,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1386,7 +1502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1400,7 +1516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1414,18 +1530,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
     <sortCondition ref="E2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1440,11 +1556,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
@@ -1452,7 +1568,7 @@
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25">
+    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -1464,7 +1580,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="17.25">
+    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -1476,7 +1592,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1487,7 +1603,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25">
+    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -1499,7 +1615,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="17.25">
+    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1511,7 +1627,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="17.25">
+    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1523,7 +1639,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1534,7 +1650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25">
+    <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>41</v>
       </c>
@@ -1546,7 +1662,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
@@ -1557,7 +1673,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.25">
+    <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -1569,7 +1685,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -1580,7 +1696,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25">
+    <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
@@ -1592,7 +1708,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>51</v>
       </c>
@@ -1603,7 +1719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.25">
+    <row r="14" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
@@ -1615,7 +1731,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -1626,10 +1742,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.25">
+    <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>57</v>
       </c>
@@ -1637,7 +1753,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -1648,7 +1764,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>62</v>
       </c>
@@ -1656,7 +1772,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>64</v>
       </c>
@@ -1664,7 +1780,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>66</v>
       </c>
@@ -1672,7 +1788,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>68</v>
       </c>
@@ -1680,17 +1796,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -1698,7 +1814,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>73</v>
       </c>
@@ -1709,7 +1825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>76</v>
       </c>
@@ -1722,316 +1838,368 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="15"/>
+    <col min="3" max="3" width="15.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="15"/>
+    <col min="7" max="7" width="17.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="24" t="s">
         <v>78</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="24" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="29"/>
-      <c r="B2" s="27" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="50">
+        <v>1</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="29">
         <v>5</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="30">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="51"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="20">
+        <v>5</v>
+      </c>
+      <c r="D3" s="21">
+        <v>3</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="30"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="17">
+      <c r="G3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="20">
         <v>5</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D4" s="21">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E4" s="22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="30"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="17">
+      <c r="G4" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="23">
         <v>5</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D5" s="32">
+        <v>5</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="27">
+        <f>SUM(D2:D21)</f>
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="47">
+        <v>2</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="34">
         <v>3</v>
       </c>
-      <c r="E4" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="31"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="17">
+      <c r="D6" s="35">
+        <v>10</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="37">
+        <v>3</v>
+      </c>
+      <c r="D7" s="38">
+        <v>3</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="50">
+        <v>3</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="29">
         <v>5</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D8" s="30">
         <v>5</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="29"/>
-      <c r="B6" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="17">
+      <c r="E8" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="20">
+        <v>5</v>
+      </c>
+      <c r="D9" s="21">
         <v>3</v>
       </c>
-      <c r="D6" s="16">
-        <v>10</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="31"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="17">
-        <v>3</v>
-      </c>
-      <c r="D7" s="16">
-        <v>3</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="29"/>
-      <c r="B8" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="17">
+      <c r="E9" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="20">
         <v>5</v>
       </c>
-      <c r="D8" s="16">
-        <v>5</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="30"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="17">
-        <v>5</v>
-      </c>
-      <c r="D9" s="16">
-        <v>3</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="30"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="17">
-        <v>5</v>
-      </c>
-      <c r="D10" s="16">
+      <c r="D10" s="21">
         <v>3</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="31"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="17">
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="23">
         <v>5</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="32">
         <v>8</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="21"/>
-      <c r="B12" s="17" t="s">
+      <c r="G11" s="18"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="55">
+        <v>4</v>
+      </c>
+      <c r="B12" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="42">
         <v>5</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="41">
         <v>8</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="40" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="29"/>
-      <c r="B13" s="27" t="s">
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="50">
+        <v>5</v>
+      </c>
+      <c r="B13" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="29">
         <v>5</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="30">
         <v>7</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="31" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="30"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="17">
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="20">
         <v>5</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="21">
         <v>15</v>
       </c>
       <c r="E14" s="22" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="30"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="17">
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="20">
         <v>5</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="21">
         <v>20</v>
       </c>
       <c r="E15" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="53"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="23">
+        <v>5</v>
+      </c>
+      <c r="D16" s="32">
+        <v>30</v>
+      </c>
+      <c r="E16" s="33" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="31"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="17">
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="54">
+        <v>6</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="34">
+        <v>3</v>
+      </c>
+      <c r="D17" s="35">
+        <v>40</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="43">
+        <v>2</v>
+      </c>
+      <c r="D18" s="44">
+        <v>30</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="43">
+        <v>2</v>
+      </c>
+      <c r="D19" s="44">
+        <v>3</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="18"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="48"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="43">
+        <v>1</v>
+      </c>
+      <c r="D20" s="44">
+        <v>15</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="37">
         <v>5</v>
       </c>
-      <c r="D16" s="16">
-        <v>30</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="29"/>
-      <c r="B17" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="17">
-        <v>3</v>
-      </c>
-      <c r="D17" s="16">
-        <v>40</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="30"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="17">
-        <v>2</v>
-      </c>
-      <c r="D18" s="16">
-        <v>30</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="30"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="17">
-        <v>2</v>
-      </c>
-      <c r="D19" s="16">
-        <v>3</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="30"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="17">
-        <v>1</v>
-      </c>
-      <c r="D20" s="16">
-        <v>15</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A21" s="32"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="25">
-        <v>5</v>
-      </c>
-      <c r="D21" s="23">
+      <c r="D21" s="38">
         <v>24</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="46" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="D22" s="15">
-        <f>SUM(D2:D21)</f>
-        <v>238</v>
-      </c>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2047,5 +2215,6 @@
     <mergeCell ref="B13:B16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
criacao da planilha de riscos
</commit_message>
<xml_diff>
--- a/documentacao/Planilha_De_Requisitos.xlsx
+++ b/documentacao/Planilha_De_Requisitos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Documents\git PI\Ar Condicionado\TechHumi\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBCB369-7DD0-4E5D-A257-434A3DAA0F44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936A2953-F61E-481D-8775-FAD4066E840A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -878,6 +878,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="7" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -900,9 +903,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,6 +1065,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:D10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D10">
+    <sortCondition descending="1" ref="C1:C10"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descrição" dataDxfId="2"/>
@@ -1374,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,13 +1412,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6">
         <v>5</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1423,13 +1426,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1437,13 +1440,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C4" s="6">
         <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1451,13 +1454,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C5" s="6">
         <v>5</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,13 +1468,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1493,13 +1496,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,13 +1510,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1521,13 +1524,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1840,7 +1843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1874,10 +1877,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="50">
+      <c r="A2" s="51">
         <v>1</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="29">
@@ -1892,8 +1895,8 @@
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51"/>
-      <c r="B3" s="51"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="20">
         <v>5</v>
       </c>
@@ -1906,8 +1909,8 @@
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="51"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="20">
         <v>5</v>
       </c>
@@ -1922,8 +1925,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
       <c r="C5" s="23">
         <v>5</v>
       </c>
@@ -1939,10 +1942,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="47">
+      <c r="A6" s="48">
         <v>2</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="48" t="s">
         <v>85</v>
       </c>
       <c r="C6" s="34">
@@ -1957,8 +1960,8 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="37">
         <v>3</v>
       </c>
@@ -1971,10 +1974,10 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="50">
+      <c r="A8" s="51">
         <v>3</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>88</v>
       </c>
       <c r="C8" s="29">
@@ -1989,8 +1992,8 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="20">
         <v>5</v>
       </c>
@@ -2003,8 +2006,8 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="20">
         <v>5</v>
       </c>
@@ -2017,8 +2020,8 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
       <c r="C11" s="23">
         <v>5</v>
       </c>
@@ -2031,7 +2034,7 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55">
+      <c r="A12" s="47">
         <v>4</v>
       </c>
       <c r="B12" s="41" t="s">
@@ -2049,10 +2052,10 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="50">
+      <c r="A13" s="51">
         <v>5</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="51" t="s">
         <v>50</v>
       </c>
       <c r="C13" s="29">
@@ -2067,8 +2070,8 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="20">
         <v>5</v>
       </c>
@@ -2081,8 +2084,8 @@
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
       <c r="C15" s="20">
         <v>5</v>
       </c>
@@ -2095,8 +2098,8 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="53"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="53"/>
       <c r="C16" s="23">
         <v>5</v>
       </c>
@@ -2109,10 +2112,10 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="54">
+      <c r="A17" s="55">
         <v>6</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="48" t="s">
         <v>99</v>
       </c>
       <c r="C17" s="34">
@@ -2127,8 +2130,8 @@
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="48"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="43">
         <v>2</v>
       </c>
@@ -2141,8 +2144,8 @@
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="43">
         <v>2</v>
       </c>
@@ -2155,8 +2158,8 @@
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="43">
         <v>1</v>
       </c>
@@ -2169,8 +2172,8 @@
       <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
-      <c r="B21" s="49"/>
+      <c r="A21" s="50"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="37">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Consertei erros ortográficos nas planilhas @esteves-esta
</commit_message>
<xml_diff>
--- a/documentacao/Planilha_De_Requisitos.xlsx
+++ b/documentacao/Planilha_De_Requisitos.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Documents\git PI\Ar Condicionado\TechHumi\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ARQUIVOS\TechHumi\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936A2953-F61E-481D-8775-FAD4066E840A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
     <sheet name="Requisitos" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint Backlog" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,9 +55,6 @@
     <t>Recuperar senha</t>
   </si>
   <si>
-    <t>Recuperação de senha atraves de email.</t>
-  </si>
-  <si>
     <t>Armazenar dados</t>
   </si>
   <si>
@@ -74,9 +70,6 @@
     <t>Controle de Temperatura e Umidade</t>
   </si>
   <si>
-    <t>Automatização do controle da temperatura e umidade atesvez de sensores</t>
-  </si>
-  <si>
     <t>Manutenção</t>
   </si>
   <si>
@@ -92,9 +85,6 @@
     <t>Programação de Horário</t>
   </si>
   <si>
-    <t>Programação opcional de horarios de funciomento da solução.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Site Adaptavel </t>
   </si>
   <si>
@@ -146,9 +136,6 @@
     <t>RNF01</t>
   </si>
   <si>
-    <t>Disponibilidade de ar condicionado na residência</t>
-  </si>
-  <si>
     <t>Desejado</t>
   </si>
   <si>
@@ -161,15 +148,9 @@
     <t>RNF03</t>
   </si>
   <si>
-    <t>Disponibilidade de umidificador de ar na residência</t>
-  </si>
-  <si>
     <t>RNF04</t>
   </si>
   <si>
-    <t>Disponibilidade de uma rede de banda larga na residência</t>
-  </si>
-  <si>
     <t>RNF05</t>
   </si>
   <si>
@@ -179,9 +160,6 @@
     <t>RNF06</t>
   </si>
   <si>
-    <t>Disponibilidade de energia elétrica na residência</t>
-  </si>
-  <si>
     <t>RNF07</t>
   </si>
   <si>
@@ -278,9 +256,6 @@
     <t>ATIVIDADE</t>
   </si>
   <si>
-    <t>Cadasrar login e senha no banco de dados</t>
-  </si>
-  <si>
     <t>Gerar login e senha automaticamente</t>
   </si>
   <si>
@@ -311,9 +286,6 @@
     <t>Criação de Tabelas do Banco de Dados</t>
   </si>
   <si>
-    <t>Con. Com o sistema</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hospedagem </t>
   </si>
   <si>
@@ -326,9 +298,6 @@
     <t>Montar a solução</t>
   </si>
   <si>
-    <t>Con. Com o banco de dados para armazenar os dados recolhidos</t>
-  </si>
-  <si>
     <t>Programar para manter a temperatura e umidade nos niveis ideias</t>
   </si>
   <si>
@@ -344,19 +313,49 @@
     <t>Formulário para suporte de clientes</t>
   </si>
   <si>
-    <t>Programação de horaro de funcionamento da solução</t>
-  </si>
-  <si>
     <t>Graficos e Analtics</t>
   </si>
   <si>
     <t>Total horas gastas:</t>
+  </si>
+  <si>
+    <t>Disponibilidade de ar condicionado nos ambientes da empresa</t>
+  </si>
+  <si>
+    <t>Disponibilidade de umidificador de ar nos ambientes da empresa</t>
+  </si>
+  <si>
+    <t>Disponibilidade de uma rede de banda larga na empresa</t>
+  </si>
+  <si>
+    <t>Disponibilidade de energia elétrica na empresa</t>
+  </si>
+  <si>
+    <t>Cadastrar login e senha no banco de dados</t>
+  </si>
+  <si>
+    <t>Conexão com o sistema</t>
+  </si>
+  <si>
+    <t>Conexão com o banco de dados para armazenar os dados recolhidos</t>
+  </si>
+  <si>
+    <t>Programação de horario de funcionamento da solução</t>
+  </si>
+  <si>
+    <t>Automatização do controle da temperatura e umidade através de sensores</t>
+  </si>
+  <si>
+    <t>Recuperação de senha através de email.</t>
+  </si>
+  <si>
+    <t>Programação opcional de horarios de funcionamento da solução.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -776,7 +775,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
@@ -905,6 +904,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="7" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Ênfase2" xfId="7" builtinId="34"/>
@@ -1063,16 +1065,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="A1:D10"/>
+  <sortState ref="A2:D10">
     <sortCondition descending="1" ref="C1:C10"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descrição" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Importancia" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Detalhe" dataDxfId="0"/>
+    <tableColumn id="1" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" name="Descrição" dataDxfId="2"/>
+    <tableColumn id="3" name="Importancia" dataDxfId="1"/>
+    <tableColumn id="5" name="Detalhe" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1374,11 +1376,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,13 +1414,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6">
         <v>5</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1426,13 +1428,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6">
         <v>5</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1440,13 +1442,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6">
         <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1474,7 +1476,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1482,13 +1484,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6">
         <v>3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1496,13 +1498,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6">
         <v>3</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1510,13 +1512,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="6">
         <v>2</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1524,27 +1526,27 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F12">
+  <sortState ref="A2:F12">
     <sortCondition ref="E2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1556,193 +1558,193 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" customWidth="1"/>
     <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
@@ -1750,87 +1752,87 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1840,11 +1842,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,7 +1855,7 @@
     <col min="2" max="2" width="34.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.85546875" style="15" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="15"/>
     <col min="7" max="7" width="17.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="15"/>
@@ -1864,16 +1866,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1890,7 +1892,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G2" s="18"/>
     </row>
@@ -1903,8 +1905,8 @@
       <c r="D3" s="21">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>81</v>
+      <c r="E3" s="56" t="s">
+        <v>99</v>
       </c>
       <c r="G3" s="18"/>
     </row>
@@ -1918,10 +1920,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1934,7 +1936,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G5" s="27">
         <f>SUM(D2:D21)</f>
@@ -1946,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C6" s="34">
         <v>3</v>
@@ -1955,7 +1957,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G6" s="18"/>
     </row>
@@ -1969,7 +1971,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G7" s="18"/>
     </row>
@@ -1978,7 +1980,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C8" s="29">
         <v>5</v>
@@ -1987,7 +1989,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G8" s="18"/>
     </row>
@@ -2001,7 +2003,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G9" s="18"/>
     </row>
@@ -2015,7 +2017,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G10" s="18"/>
     </row>
@@ -2028,8 +2030,8 @@
       <c r="D11" s="32">
         <v>8</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>92</v>
+      <c r="E11" s="57" t="s">
+        <v>100</v>
       </c>
       <c r="G11" s="18"/>
     </row>
@@ -2038,7 +2040,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C12" s="42">
         <v>5</v>
@@ -2047,7 +2049,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G12" s="18"/>
     </row>
@@ -2056,7 +2058,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C13" s="29">
         <v>5</v>
@@ -2065,7 +2067,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G13" s="18"/>
     </row>
@@ -2079,7 +2081,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="G14" s="18"/>
     </row>
@@ -2093,7 +2095,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G15" s="18"/>
     </row>
@@ -2106,8 +2108,8 @@
       <c r="D16" s="32">
         <v>30</v>
       </c>
-      <c r="E16" s="33" t="s">
-        <v>97</v>
+      <c r="E16" s="57" t="s">
+        <v>101</v>
       </c>
       <c r="G16" s="18"/>
     </row>
@@ -2116,7 +2118,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C17" s="34">
         <v>3</v>
@@ -2125,7 +2127,7 @@
         <v>40</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="G17" s="18"/>
     </row>
@@ -2139,7 +2141,7 @@
         <v>30</v>
       </c>
       <c r="E18" s="45" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="G18" s="18"/>
     </row>
@@ -2153,7 +2155,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="45" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G19" s="18"/>
     </row>
@@ -2166,8 +2168,8 @@
       <c r="D20" s="44">
         <v>15</v>
       </c>
-      <c r="E20" s="45" t="s">
-        <v>103</v>
+      <c r="E20" s="58" t="s">
+        <v>102</v>
       </c>
       <c r="G20" s="18"/>
     </row>
@@ -2181,7 +2183,7 @@
         <v>24</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G21" s="18"/>
     </row>

</xml_diff>

<commit_message>
alteração na planilha de riscos @esteves-esta
</commit_message>
<xml_diff>
--- a/documentacao/Planilha_De_Requisitos.xlsx
+++ b/documentacao/Planilha_De_Requisitos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="2" r:id="rId1"/>
@@ -880,33 +880,33 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Ênfase2" xfId="7" builtinId="34"/>
@@ -1066,7 +1066,12 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:D10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:D10"/>
+  <autoFilter ref="A1:D10">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
   <sortState ref="A2:D10">
     <sortCondition descending="1" ref="C1:C10"/>
   </sortState>
@@ -1379,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1845,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,10 +1884,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="51">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="54" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="29">
@@ -1897,22 +1902,22 @@
       <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
       <c r="C3" s="20">
         <v>5</v>
       </c>
       <c r="D3" s="21">
         <v>3</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="48" t="s">
         <v>99</v>
       </c>
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="20">
         <v>5</v>
       </c>
@@ -1927,8 +1932,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="23">
         <v>5</v>
       </c>
@@ -1944,10 +1949,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="48">
+      <c r="A6" s="51">
         <v>2</v>
       </c>
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="51" t="s">
         <v>77</v>
       </c>
       <c r="C6" s="34">
@@ -1962,8 +1967,8 @@
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="37">
         <v>3</v>
       </c>
@@ -1976,10 +1981,10 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="51">
+      <c r="A8" s="54">
         <v>3</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="54" t="s">
         <v>80</v>
       </c>
       <c r="C8" s="29">
@@ -1994,8 +1999,8 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="55"/>
+      <c r="B9" s="55"/>
       <c r="C9" s="20">
         <v>5</v>
       </c>
@@ -2008,8 +2013,8 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="55"/>
       <c r="C10" s="20">
         <v>5</v>
       </c>
@@ -2022,15 +2027,15 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="23">
         <v>5</v>
       </c>
       <c r="D11" s="32">
         <v>8</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="49" t="s">
         <v>100</v>
       </c>
       <c r="G11" s="18"/>
@@ -2054,10 +2059,10 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="51">
+      <c r="A13" s="54">
         <v>5</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="54" t="s">
         <v>43</v>
       </c>
       <c r="C13" s="29">
@@ -2072,8 +2077,8 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="20">
         <v>5</v>
       </c>
@@ -2086,8 +2091,8 @@
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="20">
         <v>5</v>
       </c>
@@ -2100,24 +2105,24 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="53"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="23">
         <v>5</v>
       </c>
       <c r="D16" s="32">
         <v>30</v>
       </c>
-      <c r="E16" s="57" t="s">
+      <c r="E16" s="49" t="s">
         <v>101</v>
       </c>
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="55">
+      <c r="A17" s="58">
         <v>6</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="51" t="s">
         <v>89</v>
       </c>
       <c r="C17" s="34">
@@ -2132,8 +2137,8 @@
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="43">
         <v>2</v>
       </c>
@@ -2146,8 +2151,8 @@
       <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
       <c r="C19" s="43">
         <v>2</v>
       </c>
@@ -2160,22 +2165,22 @@
       <c r="G19" s="18"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
       <c r="C20" s="43">
         <v>1</v>
       </c>
       <c r="D20" s="44">
         <v>15</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="50" t="s">
         <v>102</v>
       </c>
       <c r="G20" s="18"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="53"/>
       <c r="C21" s="37">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
arrumei erro ortogrfico na planilha
</commit_message>
<xml_diff>
--- a/documentacao/Planilha_De_Requisitos.xlsx
+++ b/documentacao/Planilha_De_Requisitos.xlsx
@@ -268,9 +268,6 @@
     <t>Alteração de Perfil</t>
   </si>
   <si>
-    <t>Redefinir de senha</t>
-  </si>
-  <si>
     <t>Alterar login e senha</t>
   </si>
   <si>
@@ -350,6 +347,9 @@
   </si>
   <si>
     <t>Programação opcional de horarios de funcionamento da solução.</t>
+  </si>
+  <si>
+    <t>Redefinição de senha</t>
   </si>
 </sst>
 </file>
@@ -775,7 +775,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="3" applyBorder="1"/>
@@ -907,6 +907,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="7" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Ênfase2" xfId="7" builtinId="34"/>
@@ -1453,7 +1454,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1481,7 +1482,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1642,7 +1643,7 @@
         <v>33</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>34</v>
@@ -1665,7 +1666,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>25</v>
@@ -1677,7 +1678,7 @@
         <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>25</v>
@@ -1700,7 +1701,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>25</v>
@@ -1851,7 +1852,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,7 +1912,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="18"/>
     </row>
@@ -1928,7 +1929,7 @@
         <v>74</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1961,8 +1962,8 @@
       <c r="D6" s="35">
         <v>10</v>
       </c>
-      <c r="E6" s="36" t="s">
-        <v>78</v>
+      <c r="E6" s="59" t="s">
+        <v>105</v>
       </c>
       <c r="G6" s="18"/>
     </row>
@@ -1976,7 +1977,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="18"/>
     </row>
@@ -1985,7 +1986,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="29">
         <v>5</v>
@@ -1994,7 +1995,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="18"/>
     </row>
@@ -2008,7 +2009,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" s="18"/>
     </row>
@@ -2022,7 +2023,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G10" s="18"/>
     </row>
@@ -2036,7 +2037,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="18"/>
     </row>
@@ -2045,7 +2046,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="42">
         <v>5</v>
@@ -2054,7 +2055,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="18"/>
     </row>
@@ -2072,7 +2073,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G13" s="18"/>
     </row>
@@ -2086,7 +2087,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="18"/>
     </row>
@@ -2100,7 +2101,7 @@
         <v>20</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="18"/>
     </row>
@@ -2114,7 +2115,7 @@
         <v>30</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="18"/>
     </row>
@@ -2123,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="34">
         <v>3</v>
@@ -2132,7 +2133,7 @@
         <v>40</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G17" s="18"/>
     </row>
@@ -2146,7 +2147,7 @@
         <v>30</v>
       </c>
       <c r="E18" s="45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G18" s="18"/>
     </row>
@@ -2160,7 +2161,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G19" s="18"/>
     </row>
@@ -2174,7 +2175,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G20" s="18"/>
     </row>
@@ -2188,7 +2189,7 @@
         <v>24</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G21" s="18"/>
     </row>

</xml_diff>